<commit_message>
update por via das duvidas
</commit_message>
<xml_diff>
--- a/teste-db.xlsx
+++ b/teste-db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\estadio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\qualestadio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E89312-6964-4C2E-BCC4-6CEB7331A41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6452739B-0FA7-4A9D-9C45-64E787026CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EADE664B-2A57-4964-8807-E6F34DBD3F9C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="226">
   <si>
     <t>Nome Oficial</t>
   </si>
@@ -389,19 +389,349 @@
   </si>
   <si>
     <t>Poções</t>
+  </si>
+  <si>
+    <t>Dica1</t>
+  </si>
+  <si>
+    <t>Dica2</t>
+  </si>
+  <si>
+    <t>Dica3</t>
+  </si>
+  <si>
+    <t>Dica4</t>
+  </si>
+  <si>
+    <t>Dica5</t>
+  </si>
+  <si>
+    <t>Foi inaugurado em 1966, numa partida entre Flamengo x Vasco.</t>
+  </si>
+  <si>
+    <t>O mascote do principal time mandante no estádio é um bode.</t>
+  </si>
+  <si>
+    <t>O recorde de público do estádio é de 15.728 pessoas, num jogo do Vitória, em janeiro de 2007.</t>
+  </si>
+  <si>
+    <t>O estádio é considerado um dos mais bonitos da Bahia e já recebeu duas finais de Baianão.</t>
+  </si>
+  <si>
+    <t>O nome do estádio é em homenagem a um ex-governador do Estado da Bahia.</t>
+  </si>
+  <si>
+    <t>É do governo estadual, mas sua administração foi cedida para a prefeitura até 2034</t>
+  </si>
+  <si>
+    <t>No dia que o estádio bateu recorde de público, o time da casa perdeu de 7x0</t>
+  </si>
+  <si>
+    <t>Foi sede da primeira edição dos Jogos Mundiais dos Povos Indígenas</t>
+  </si>
+  <si>
+    <t>Em sua área fica também o Kartódromo Rubens Barrichello e a Vila Olímpica Indígena</t>
+  </si>
+  <si>
+    <t>Recebe o nome do lateral esquerdo da seleção bi-campeã do mundo em 1962</t>
+  </si>
+  <si>
+    <t>O primeiro gol foi marcado pelo jogador Paraná</t>
+  </si>
+  <si>
+    <t>Já foi palco de uma semifinal de Brasileirão</t>
+  </si>
+  <si>
+    <t>A capacidade é de aproximadamente 30 mil pessoas</t>
+  </si>
+  <si>
+    <t>Fica na região Sul do país</t>
+  </si>
+  <si>
+    <t>O nome do estádio faz referência a uma bebida</t>
+  </si>
+  <si>
+    <t>Foi palco do gol mais rápido da história da Série A</t>
+  </si>
+  <si>
+    <t>Foi palco de uma das mais históricas partidas da Série B</t>
+  </si>
+  <si>
+    <t>Em 2013, deixou de ser usado pelo time da casa, que passou a jogar em uma arena da Copa 2014</t>
+  </si>
+  <si>
+    <t>Anos depois, após campanha da torcida, o clube da casa voltou a jogar aqui</t>
+  </si>
+  <si>
+    <t>Seu maior público foi na final do Campeonato Estadual de 1970</t>
+  </si>
+  <si>
+    <t>A primeira partida foi em 1953, mas a iluminação só foi inaugurada 11 anos depois</t>
+  </si>
+  <si>
+    <t>O time dono do estádio é um campeão brasileiro</t>
+  </si>
+  <si>
+    <t>Na Copa 2014, foi usado para treinos pela seleção da Nigéria</t>
+  </si>
+  <si>
+    <t>Fica numa cidade cujo apelido é Princesa d'Oeste</t>
+  </si>
+  <si>
+    <t>Foi palco da partida final do Campeonato Brasileiro de 1978 e 1986</t>
+  </si>
+  <si>
+    <t>Fica em uma cidade no interior da região Sul</t>
+  </si>
+  <si>
+    <t>O clube dono da casa ficou praticamente 10 anos licenciado, entre as décadas de 1990 e 2000</t>
+  </si>
+  <si>
+    <t>O nome do estádio homenageia um engenheiro ferroviária que elaborou o plano para construção da arena</t>
+  </si>
+  <si>
+    <t>O estádio foi construído perto de uma linha de trem, que era usada para o transporte dos materiais de construção</t>
+  </si>
+  <si>
+    <t>Foi palco da final da Série D de 2017, quando o time da casa foi campeão</t>
+  </si>
+  <si>
+    <t>Foi inaugurado em 1980, mas passou por amplas reformas entre 2008 e 2009</t>
+  </si>
+  <si>
+    <t>O autor do primeiro gol foi Bira, atacante do Internacional</t>
+  </si>
+  <si>
+    <t>A capacidade do estádio é de cerca de 20 mil torcedores</t>
+  </si>
+  <si>
+    <t>O nome do estádio homenageia um líder indígena kaingang</t>
+  </si>
+  <si>
+    <t>Teria sido palco de uma final de Copa Sul-Americana se não fosse por um trágico acidente</t>
+  </si>
+  <si>
+    <t>Quatro vezes o estádio viu o placar marcar 7x0, sempre com vitória do time da casa</t>
+  </si>
+  <si>
+    <t>A construção contou com apoio do governador João Durval Carneiro, que homenageou o sogro com o nome do estádio</t>
+  </si>
+  <si>
+    <t>Flávio Tanajura atuou 107 vezes neste estádio, mas o artilheiro é Neto Baiano, com 53 gols em 4 temporadas</t>
+  </si>
+  <si>
+    <t>Em 2000 o estádio recebeu 51.200 espectadores durante vitória do time da casa sobre o Juazeiro</t>
+  </si>
+  <si>
+    <t>O clube dono deste estádio chegou a uma final do Campeonato Brasileiro, mas mandou o jogo decisivo em um estádio maior na mesma cidade</t>
+  </si>
+  <si>
+    <t>Originalmente, o estádio ia levar o nome do governador, mas o sucesso do Brasil na Copa de 1970 fez com que os planos mudassem</t>
+  </si>
+  <si>
+    <t>Os times que mandam seus jogos aqui geralmente são chamados por suas siglas</t>
+  </si>
+  <si>
+    <t>O nome do estádio homageia um jogador cujo clube participou da partida inaugural. Na ocasião, ele fez dois gols</t>
+  </si>
+  <si>
+    <t>Hoje, tem capacidade para cerca de 20 mil pessoas</t>
+  </si>
+  <si>
+    <t>Também é conhecido como "Trapichão"</t>
+  </si>
+  <si>
+    <t>Foi construído para a disputa da Copa de 1950</t>
+  </si>
+  <si>
+    <t>É o segundo principal estádio da cidade onde está localizado</t>
+  </si>
+  <si>
+    <t>No início da década de 2010, o estádio foi demolido quase na íntegra e outro foi construído no mesmo lugar</t>
+  </si>
+  <si>
+    <t>Pertenceu a um clube chamado Sete de Setembro, razão de ter ficado conhecido pelo nome atual</t>
+  </si>
+  <si>
+    <t>Foi aqui que o goleiro Victor fez uma defesa que foi imortalizada em cantos da torcida do Galo</t>
+  </si>
+  <si>
+    <t>O nome é uma homenagem ao homem que construiu o estádios com recursos próprios</t>
+  </si>
+  <si>
+    <t>A capacidade atual do estádio é de 16 mil, mas já recebeu quase 23 mil pessoas na final de um estadual</t>
+  </si>
+  <si>
+    <t>O dono original da casa foi um clube extinto em 1999</t>
+  </si>
+  <si>
+    <t>Em 2010, um novo time foi fundado mantendo as cores e a identidade visual do anterior</t>
+  </si>
+  <si>
+    <t>O estádio foi inaugurado em março de 1987 com a derrota do time da casa para o Inter de Limeira</t>
+  </si>
+  <si>
+    <t>A inauguração do estádio foi em um jogo amistoso contra o Internacional em 1980, que terminou empatado em 2 x 2</t>
+  </si>
+  <si>
+    <t>É o estádio do último time do ex-jogador Danilo, campeão Mundial pelo Corinthians em 2012</t>
+  </si>
+  <si>
+    <t>É a casa de um dos três grandes times da cidade</t>
+  </si>
+  <si>
+    <t>Túlio Maravilha, defendendo o time da casa, já fez quatro gols em um único jogo aqui</t>
+  </si>
+  <si>
+    <t>O Botafogo estreou na Série B de 2021 nesse estádio</t>
+  </si>
+  <si>
+    <t>Imagem</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>24.jpg</t>
+  </si>
+  <si>
+    <t>19.jpg</t>
+  </si>
+  <si>
+    <t>1.jpg</t>
+  </si>
+  <si>
+    <t>2.jpg</t>
+  </si>
+  <si>
+    <t>3.jpg</t>
+  </si>
+  <si>
+    <t>4.jpg</t>
+  </si>
+  <si>
+    <t>5.jpg</t>
+  </si>
+  <si>
+    <t>6.jpg</t>
+  </si>
+  <si>
+    <t>7.jpg</t>
+  </si>
+  <si>
+    <t>8.jpg</t>
+  </si>
+  <si>
+    <t>9.jpg</t>
+  </si>
+  <si>
+    <t>10.jpg</t>
+  </si>
+  <si>
+    <t>11.jpg</t>
+  </si>
+  <si>
+    <t>12.jpg</t>
+  </si>
+  <si>
+    <t>13.jpg</t>
+  </si>
+  <si>
+    <t>14.jpg</t>
+  </si>
+  <si>
+    <t>15.jpg</t>
+  </si>
+  <si>
+    <t>16.jpg</t>
+  </si>
+  <si>
+    <t>17.jpg</t>
+  </si>
+  <si>
+    <t>18.jpg</t>
+  </si>
+  <si>
+    <t>20.jpg</t>
+  </si>
+  <si>
+    <t>21.jpg</t>
+  </si>
+  <si>
+    <t>22.jpg</t>
+  </si>
+  <si>
+    <t>23.jpg</t>
+  </si>
+  <si>
+    <t>25.jpg</t>
+  </si>
+  <si>
+    <t>26.jpg</t>
+  </si>
+  <si>
+    <t>27.jpg</t>
+  </si>
+  <si>
+    <t>28.jpg</t>
+  </si>
+  <si>
+    <t>29.jpg</t>
+  </si>
+  <si>
+    <t>30.jpg</t>
+  </si>
+  <si>
+    <t>31.jpg</t>
+  </si>
+  <si>
+    <t>32.jpg</t>
+  </si>
+  <si>
+    <t>33.jpg</t>
+  </si>
+  <si>
+    <t>34.jpg</t>
+  </si>
+  <si>
+    <t>35.jpg</t>
+  </si>
+  <si>
+    <t>36.jpg</t>
+  </si>
+  <si>
+    <t>37.jpg</t>
+  </si>
+  <si>
+    <t>38.jpg</t>
+  </si>
+  <si>
+    <t>39.jpg</t>
+  </si>
+  <si>
+    <t>40.jpg</t>
+  </si>
+  <si>
+    <t>41.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -421,14 +751,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{4415B4D7-E736-435C-8765-F1457637798C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -740,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F76165-F908-4EDA-A543-F983FA1DAFA9}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,9 +1096,15 @@
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -766,8 +1117,29 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -780,8 +1152,14 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>187</v>
+      </c>
+      <c r="K2" s="12">
+        <v>44723</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -794,8 +1172,14 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3" s="12">
+        <v>44724</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -808,8 +1192,14 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" s="12">
+        <v>44725</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -822,8 +1212,14 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" s="12">
+        <v>44726</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -836,8 +1232,29 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="K6" s="12">
+        <v>44727</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -850,8 +1267,14 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>192</v>
+      </c>
+      <c r="K7" s="12">
+        <v>44728</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -864,8 +1287,14 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>193</v>
+      </c>
+      <c r="K8" s="12">
+        <v>44729</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -878,8 +1307,14 @@
       <c r="D9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>194</v>
+      </c>
+      <c r="K9" s="12">
+        <v>44730</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -892,8 +1327,14 @@
       <c r="D10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>195</v>
+      </c>
+      <c r="K10" s="12">
+        <v>44731</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -906,8 +1347,14 @@
       <c r="D11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>196</v>
+      </c>
+      <c r="K11" s="12">
+        <v>44732</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -920,8 +1367,29 @@
       <c r="D12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="K12" s="12">
+        <v>44733</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -934,8 +1402,14 @@
       <c r="D13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>198</v>
+      </c>
+      <c r="K13" s="12">
+        <v>44734</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -948,8 +1422,14 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>199</v>
+      </c>
+      <c r="K14" s="12">
+        <v>44735</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -962,8 +1442,14 @@
       <c r="D15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>200</v>
+      </c>
+      <c r="K15" s="12">
+        <v>44736</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -976,8 +1462,14 @@
       <c r="D16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>201</v>
+      </c>
+      <c r="K16" s="12">
+        <v>44737</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -990,8 +1482,14 @@
       <c r="D17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>202</v>
+      </c>
+      <c r="K17" s="12">
+        <v>44738</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1004,8 +1502,14 @@
       <c r="D18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>203</v>
+      </c>
+      <c r="K18" s="12">
+        <v>44739</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1018,8 +1522,29 @@
       <c r="D19" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G19" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" t="s">
+        <v>204</v>
+      </c>
+      <c r="K19" s="12">
+        <v>44740</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1032,8 +1557,14 @@
       <c r="D20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>186</v>
+      </c>
+      <c r="K20" s="12">
+        <v>44741</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1046,8 +1577,14 @@
       <c r="D21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>205</v>
+      </c>
+      <c r="K21" s="12">
+        <v>44742</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1060,8 +1597,14 @@
       <c r="D22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>206</v>
+      </c>
+      <c r="K22" s="12">
+        <v>44743</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1074,8 +1617,14 @@
       <c r="D23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>207</v>
+      </c>
+      <c r="K23" s="12">
+        <v>44744</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -1088,8 +1637,29 @@
       <c r="D24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="K24" s="12">
+        <v>44745</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -1102,8 +1672,29 @@
       <c r="D25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K25" s="12">
+        <v>44746</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1116,8 +1707,29 @@
       <c r="D26" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="K26" s="12">
+        <v>44747</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -1130,8 +1742,14 @@
       <c r="D27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J27" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="K27" s="12">
+        <v>44748</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1144,8 +1762,14 @@
       <c r="D28" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J28" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="K28" s="12">
+        <v>44749</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1158,8 +1782,14 @@
       <c r="D29" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J29" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="K29" s="12">
+        <v>44750</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1172,8 +1802,29 @@
       <c r="D30" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="K30" s="12">
+        <v>44751</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -1186,8 +1837,14 @@
       <c r="D31" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J31" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="K31" s="12">
+        <v>44752</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -1200,8 +1857,14 @@
       <c r="D32" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J32" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="K32" s="12">
+        <v>44753</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -1214,8 +1877,14 @@
       <c r="D33" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J33" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="K33" s="12">
+        <v>44754</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>95</v>
       </c>
@@ -1228,8 +1897,14 @@
       <c r="D34" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J34" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="K34" s="12">
+        <v>44755</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -1242,8 +1917,29 @@
       <c r="D35" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="K35" s="12">
+        <v>44756</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -1256,8 +1952,29 @@
       <c r="D36" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="K36" s="12">
+        <v>44757</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -1270,8 +1987,14 @@
       <c r="D37" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J37" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="K37" s="12">
+        <v>44758</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -1284,8 +2007,29 @@
       <c r="D38" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="K38" s="12">
+        <v>44759</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -1298,8 +2042,29 @@
       <c r="D39" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="K39" s="12">
+        <v>44760</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>109</v>
       </c>
@@ -1312,8 +2077,29 @@
       <c r="D40" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="K40" s="12">
+        <v>44761</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -1326,8 +2112,14 @@
       <c r="D41" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J41" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="K41" s="12">
+        <v>44762</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -1340,8 +2132,15 @@
       <c r="D42" t="s">
         <v>57</v>
       </c>
+      <c r="J42" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="K42" s="12">
+        <v>44763</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>